<commit_message>
Implement validation for importing Excel workbooks
</commit_message>
<xml_diff>
--- a/Schema/template.xlsx
+++ b/Schema/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\React Budget App\Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1713E23D-A7E7-4210-963D-76D3EE09E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C55DCA-760F-44F2-A39E-7B8034D925D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A682B92-E955-49E4-9CBC-FB857D42C240}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Budgets</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Current Month:</t>
-  </si>
-  <si>
-    <t>Previous Month:</t>
   </si>
   <si>
     <t>First Monday</t>
@@ -241,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +248,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB9EDFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,203 +289,195 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="2"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="72">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -501,18 +496,58 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -535,7 +570,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -561,10 +596,10 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -587,10 +622,10 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -613,10 +648,9 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -639,10 +673,10 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -665,7 +699,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -675,223 +709,13 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
           <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -910,6 +734,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -1062,21 +887,21 @@
           <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -1102,7 +927,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1118,7 +943,7 @@
           <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1137,6 +962,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -1162,7 +988,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -1188,7 +1014,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -1214,7 +1040,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -1240,7 +1066,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -1264,7 +1090,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1289,7 +1115,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1314,7 +1140,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1330,7 +1156,7 @@
           <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1349,6 +1175,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -1372,7 +1199,7 @@
           <color auto="1"/>
         </bottom>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1397,76 +1224,76 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -1490,7 +1317,7 @@
           <color auto="1"/>
         </bottom>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1499,7 +1326,7 @@
           <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1518,13 +1345,108 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="2"/>
@@ -1563,56 +1485,54 @@
           <color auto="1"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1621,7 +1541,7 @@
           <bgColor rgb="FFB9EDFF"/>
         </patternFill>
       </fill>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1639,6 +1559,72 @@
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
+      </font>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
       </font>
     </dxf>
   </dxfs>
@@ -1661,119 +1647,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{17C888D4-D2A0-42A3-AF7A-69DDB6132627}" name="Budgets" displayName="Budgets" ref="I5:P6" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{17C888D4-D2A0-42A3-AF7A-69DDB6132627}" name="Budgets" displayName="Budgets" ref="I5:P6" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="I5:P6" xr:uid="{6993C61E-5182-4571-996F-3C4DB6F2B5F2}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{83BDF8A9-16D5-4FAD-8883-B8AB4BF0CBF9}" name="Name" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{DF4C47DB-0C38-4140-9A4F-CBFFCE84A85D}" name="Type" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{D266A9E0-9F8B-47FD-BA0B-3E60FE29E3D1}" name="Amount" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{02A995E3-B20A-4F4A-A6F7-7A14AF77ED1F}" name="Rollover From Last Month" dataDxfId="68">
-      <calculatedColumnFormula>IF(Budgets[[#This Row],[Type]]&lt;&gt;"Rolling", "", IF(NOT(ISBLANK(Budgets[[#This Row],[Override Rollover Amount]])), Budgets[[#This Row],[Override Rollover Amount]], SUMIF(INDIRECT("_" &amp; SUBSTITUTE($E$2,"-","_") &amp; "\Budgets[Name]"),Budgets[[#This Row],[Name]],INDIRECT("_" &amp; SUBSTITUTE($E$2,"-","_") &amp; "\Budgets[Remaining Budget]"))))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{ADF04C24-7619-420B-BB47-052C5B44BEF4}" name="Override Rollover Amount" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{0BB6F0D2-7D45-4C3E-9731-68F5C9C5C7B5}" name="Total Debits" dataDxfId="2">
-      <calculatedColumnFormula>SUMIFS(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Amount]"), INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Category]"),Budgets[[#This Row],[Name]], INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Type]"),"Debit")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{A939EBD1-196A-46D7-B1EA-B0874692155B}" name="Total Credits" dataDxfId="1">
-      <calculatedColumnFormula>SUMIFS(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Amount]"), INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Category]"),Budgets[[#This Row],[Name]], INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Type]"),"Credit")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{51181065-A55C-4635-93FD-180ED457A61F}" name="Remaining Budget" dataDxfId="0">
-      <calculatedColumnFormula>IF(Budgets[[#This Row],[Type]]&lt;&gt;"Saving", Budgets[[#This Row],[Amount]]+IF(NOT(Budgets[[#This Row],[Rollover From Last Month]]=""),Budgets[[#This Row],[Rollover From Last Month]],0)-Budgets[[#This Row],[Total Debits]]+Budgets[[#This Row],[Total Credits]], Budgets[[#This Row],[Amount]]+IF(NOT(Budgets[[#This Row],[Rollover From Last Month]]=""),Budgets[[#This Row],[Rollover From Last Month]],0)+Budgets[[#This Row],[Total Debits]]-Budgets[[#This Row],[Total Credits]])</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{83BDF8A9-16D5-4FAD-8883-B8AB4BF0CBF9}" name="Name" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{DF4C47DB-0C38-4140-9A4F-CBFFCE84A85D}" name="Type" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{D266A9E0-9F8B-47FD-BA0B-3E60FE29E3D1}" name="Amount" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{02A995E3-B20A-4F4A-A6F7-7A14AF77ED1F}" name="Rollover From Last Month" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{ADF04C24-7619-420B-BB47-052C5B44BEF4}" name="Override Rollover Amount" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{0BB6F0D2-7D45-4C3E-9731-68F5C9C5C7B5}" name="Total Debits" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{A939EBD1-196A-46D7-B1EA-B0874692155B}" name="Total Credits" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{51181065-A55C-4635-93FD-180ED457A61F}" name="Remaining Budget" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="57" xr:uid="{D4247360-4C75-4EEA-A4C2-8C34C5F915EF}" name="Transactions" displayName="Transactions" ref="B19:G20" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="57" xr:uid="{D4247360-4C75-4EEA-A4C2-8C34C5F915EF}" name="Transactions" displayName="Transactions" ref="B19:G20" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="B19:G20" xr:uid="{EC46B62F-7A14-4839-B25C-76E755827075}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7477D824-16EA-4400-8A4A-A26D94B0BDB2}" name="Date" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{4804B0F6-75F9-4C71-82B4-253110B76157}" name="Location" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{5ECA2053-BFE4-4C1D-B7D3-3F5BE41BA416}" name="Description" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{1D632AF3-D9F2-4D16-BAD9-56A43FE7CEDA}" name="Category" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{7496558E-9DF8-4A02-8DAB-BF4F75986351}" name="Type" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{C38D712B-2662-4B3B-A13E-3A4F0BC5BFC0}" name="Amount" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{7477D824-16EA-4400-8A4A-A26D94B0BDB2}" name="Date" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{4804B0F6-75F9-4C71-82B4-253110B76157}" name="Location" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{5ECA2053-BFE4-4C1D-B7D3-3F5BE41BA416}" name="Description" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{1D632AF3-D9F2-4D16-BAD9-56A43FE7CEDA}" name="Category" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{7496558E-9DF8-4A02-8DAB-BF4F75986351}" name="Type" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{C38D712B-2662-4B3B-A13E-3A4F0BC5BFC0}" name="Amount" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{C273FBC6-CF07-4A38-A070-C0C9DFF56067}" name="Balances" displayName="Balances" ref="I9:O10" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{C273FBC6-CF07-4A38-A070-C0C9DFF56067}" name="Balances" displayName="Balances" ref="I9:O10" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="I9:O10" xr:uid="{9874A6B0-EF6A-4DFE-B7B5-17DAD41163E3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9E5C9582-5D2F-4C0A-ADB1-B75EFE305F06}" name="Name" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{80AD80A2-4E70-45A8-91C7-AFB3CA3A6FC7}" name="Category" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{AD75D4A6-C383-4C52-858E-D0105EB0DB85}" name="First Monday" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{DC809384-94C0-4AD0-975B-7E980BFF2F3E}" name="Second Monday" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{0BEFD098-ADC6-4E9E-84D7-31A05AA1394B}" name="Third Monday" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{C9616504-7670-4B53-B90A-4D4E4EF3F460}" name="Fourth Monday" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{91176B76-109E-468C-8E43-8389F167B35D}" name="Fifth Monday" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{9E5C9582-5D2F-4C0A-ADB1-B75EFE305F06}" name="Name" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{80AD80A2-4E70-45A8-91C7-AFB3CA3A6FC7}" name="Category" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{AD75D4A6-C383-4C52-858E-D0105EB0DB85}" name="First Monday" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{DC809384-94C0-4AD0-975B-7E980BFF2F3E}" name="Second Monday" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{0BEFD098-ADC6-4E9E-84D7-31A05AA1394B}" name="Third Monday" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{C9616504-7670-4B53-B90A-4D4E4EF3F460}" name="Fourth Monday" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{91176B76-109E-468C-8E43-8389F167B35D}" name="Fifth Monday" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{09AF0EAE-135D-4830-9332-C3A0BF529D5F}" name="Expected.Income.Dates" displayName="Expected.Income.Dates" ref="I17:P18" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{09AF0EAE-135D-4830-9332-C3A0BF529D5F}" name="Expected.Income.Dates" displayName="Expected.Income.Dates" ref="I17:P18" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="I17:P18" xr:uid="{CBEC8C2F-5549-4B3F-927C-B3465789AE2F}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{FC3C485A-E65E-4BE0-A361-D221B5B9A085}" name="Date" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{D44C6079-9B01-41CF-9287-6CB7E52B791D}" name="Employer" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{E5CB86C1-FAB1-49FB-92D5-353C34491185}" name="Gross Income" dataDxfId="44">
-      <calculatedColumnFormula>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",$J$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline",#REF!, " "))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{D138DC48-B257-4C61-BF6D-F6680E974E01}" name="Retirement Contributions" dataDxfId="43">
-      <calculatedColumnFormula>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",Expected.Income.Dates[[#This Row],[Gross Income]]*$K$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline", Expected.Income.Dates[[#This Row],[Gross Income]]*#REF!, " "))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{80DCE307-B822-4242-85B2-B071132D0B68}" name="Healthcare Deductions" dataDxfId="42">
-      <calculatedColumnFormula>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",$L$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline",#REF!, " "))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{A786589B-65B8-4B4B-9E4F-DE94C70BCF44}" name="Other Payroll Deductions" dataDxfId="41">
-      <calculatedColumnFormula>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",$M$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline",#REF!, " "))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{26E76CDC-3355-4D93-B906-759D5C989E00}" name="Taxes" dataDxfId="40">
-      <calculatedColumnFormula>IF(Expected.Income.Dates[[#This Row],[Employer]]&lt;&gt; "", $N$14*(Expected.Income.Dates[[#This Row],[Gross Income]]-Expected.Income.Dates[[#This Row],[Retirement Contributions]]-Expected.Income.Dates[[#This Row],[Healthcare Deductions]]-Expected.Income.Dates[[#This Row],[Other Payroll Deductions]]), "")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{C7CDC12B-923A-445D-B779-812E489C9287}" name="Net Income" dataDxfId="39">
-      <calculatedColumnFormula>IF(Expected.Income.Dates[[#This Row],[Employer]]&lt;&gt;"", Expected.Income.Dates[[#This Row],[Gross Income]]-Expected.Income.Dates[[#This Row],[Retirement Contributions]]-Expected.Income.Dates[[#This Row],[Healthcare Deductions]]-Expected.Income.Dates[[#This Row],[Other Payroll Deductions]]-Expected.Income.Dates[[#This Row],[Taxes]], "")</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{FC3C485A-E65E-4BE0-A361-D221B5B9A085}" name="Date" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{D44C6079-9B01-41CF-9287-6CB7E52B791D}" name="Employer" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{E5CB86C1-FAB1-49FB-92D5-353C34491185}" name="Gross Income" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{D138DC48-B257-4C61-BF6D-F6680E974E01}" name="Retirement Contributions" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{80DCE307-B822-4242-85B2-B071132D0B68}" name="Healthcare Deductions" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{A786589B-65B8-4B4B-9E4F-DE94C70BCF44}" name="Other Payroll Deductions" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{26E76CDC-3355-4D93-B906-759D5C989E00}" name="Taxes" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{C7CDC12B-923A-445D-B779-812E489C9287}" name="Net Income" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="65" xr:uid="{0BD58F66-E887-4D29-9DAF-C8F7A14239A6}" name="Actual.Income" displayName="Actual.Income" ref="I21:P22" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="65" xr:uid="{0BD58F66-E887-4D29-9DAF-C8F7A14239A6}" name="Actual.Income" displayName="Actual.Income" ref="I21:P22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="I21:P22" xr:uid="{E5E28DBB-8C36-4879-9321-9B9564D6F520}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0C0B9DAD-7953-441A-84BF-6A323C85C9AC}" name="Date" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{63156741-6A32-4F93-B248-543E00DE0E35}" name="Employer" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{66130143-3A36-4DD3-911B-6EF33047C78D}" name="Gross Income" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{56CBED11-2DCE-449A-B1B5-0F87262530C2}" name="Retirement Contributions" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{3E3E4A85-604D-4BF0-8E1A-262CB28E4641}" name="Healthcare Deductions" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{AD8EF7F8-E3CD-48C3-BD5D-27B5260F6A89}" name="Other Payroll Deductions" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{7670475F-B64A-4B39-849D-FC97909C80BE}" name="Taxes" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{686A1350-5F75-406D-80B0-9C2F3E1D733B}" name="Net Income" dataDxfId="28">
-      <calculatedColumnFormula>Actual.Income[[#This Row],[Gross Income]]-Actual.Income[[#This Row],[Retirement Contributions]]-Actual.Income[[#This Row],[Healthcare Deductions]]-Actual.Income[[#This Row],[Other Payroll Deductions]]-Actual.Income[[#This Row],[Taxes]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{0C0B9DAD-7953-441A-84BF-6A323C85C9AC}" name="Date" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{63156741-6A32-4F93-B248-543E00DE0E35}" name="Employer" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{66130143-3A36-4DD3-911B-6EF33047C78D}" name="Gross Income" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{56CBED11-2DCE-449A-B1B5-0F87262530C2}" name="Retirement Contributions" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{3E3E4A85-604D-4BF0-8E1A-262CB28E4641}" name="Healthcare Deductions" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{AD8EF7F8-E3CD-48C3-BD5D-27B5260F6A89}" name="Other Payroll Deductions" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{7670475F-B64A-4B39-849D-FC97909C80BE}" name="Taxes" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{686A1350-5F75-406D-80B0-9C2F3E1D733B}" name="Net Income" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5295C20-1626-4C76-B7F1-5775E8FB9CC8}" name="Expected.Income.Rates" displayName="Expected.Income.Rates" ref="I13:N14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="20" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5295C20-1626-4C76-B7F1-5775E8FB9CC8}" name="Expected.Income.Rates" displayName="Expected.Income.Rates" ref="I13:N14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="I13:N14" xr:uid="{F5295C20-1626-4C76-B7F1-5775E8FB9CC8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0D648D37-3BFC-4802-9F99-B6A4EDE9FE0D}" name="Employer" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{64D66403-684E-479C-AF8A-A81CD459EE72}" name="Gross Income" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{83994055-BBE2-428A-ADDF-635673F5934A}" name="Retirement Contribution Rate" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{0CB4F419-FD7E-4B6C-8BBE-EC2CABC7F1C7}" name="Healthcare Deductions" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{7F7310D7-C7FC-4659-AED7-48C46DE02E0E}" name="Other Payroll Deductions" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{54ABFE45-F89F-46E6-AED9-4869937C027C}" name="Tax Rate" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{0D648D37-3BFC-4802-9F99-B6A4EDE9FE0D}" name="Employer" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{64D66403-684E-479C-AF8A-A81CD459EE72}" name="Gross Income" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{83994055-BBE2-428A-ADDF-635673F5934A}" name="Retirement Contribution Rate" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0CB4F419-FD7E-4B6C-8BBE-EC2CABC7F1C7}" name="Healthcare Deductions" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7F7310D7-C7FC-4659-AED7-48C46DE02E0E}" name="Other Payroll Deductions" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{54ABFE45-F89F-46E6-AED9-4869937C027C}" name="Tax Rate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2079,8 +2043,8 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,26 +2075,20 @@
         <f t="array" aca="1" ref="C2" ca="1">_xlfn.TEXTAFTER(CELL("filename",A1),"]")</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="e">
-        <f ca="1">_xlfn.CONCAT(IF(RIGHT(C2,2)="01", VALUE(LEFT(C2,4))-1, LEFT(C2,4)), "-", IF(RIGHT(C2,2)="01","12",TEXT(VALUE(RIGHT(C2,2))-1,"00")))</f>
-        <v>#N/A</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="4" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>0</v>
@@ -2138,17 +2096,17 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="8" t="e">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Gross Income]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D5" s="8" t="e">
+      <c r="D5" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Gross Income]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E5" s="9" t="e">
+      <c r="E5" s="4" t="e">
         <f ca="1">D5-C5</f>
         <v>#N/A</v>
       </c>
@@ -2168,10 +2126,10 @@
         <v>7</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>4</v>
@@ -2179,91 +2137,79 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="8" t="e">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Retirement Contributions]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D6" s="8" t="e">
+      <c r="D6" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Retirement Contributions]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E6" s="9" t="e">
+      <c r="E6" s="4" t="e">
         <f ca="1">D6-C6</f>
         <v>#N/A</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="10" t="str">
-        <f ca="1">IF(Budgets[[#This Row],[Type]]&lt;&gt;"Rolling", "", IF(NOT(ISBLANK(Budgets[[#This Row],[Override Rollover Amount]])), Budgets[[#This Row],[Override Rollover Amount]], SUMIF(INDIRECT("_" &amp; SUBSTITUTE($E$2,"-","_") &amp; "\Budgets[Name]"),Budgets[[#This Row],[Name]],INDIRECT("_" &amp; SUBSTITUTE($E$2,"-","_") &amp; "\Budgets[Remaining Budget]"))))</f>
-        <v/>
-      </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="13" t="e">
-        <f ca="1">SUMIFS(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Amount]"), INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Category]"),Budgets[[#This Row],[Name]], INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Type]"),"Debit")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O6" s="13" t="e">
-        <f ca="1">SUMIFS(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Amount]"), INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Category]"),Budgets[[#This Row],[Name]], INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[Type]"),"Credit")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P6" s="13" t="e">
-        <f ca="1">IF(Budgets[[#This Row],[Type]]&lt;&gt;"Saving", Budgets[[#This Row],[Amount]]+IF(NOT(Budgets[[#This Row],[Rollover From Last Month]]=""),Budgets[[#This Row],[Rollover From Last Month]],0)-Budgets[[#This Row],[Total Debits]]+Budgets[[#This Row],[Total Credits]], Budgets[[#This Row],[Amount]]+IF(NOT(Budgets[[#This Row],[Rollover From Last Month]]=""),Budgets[[#This Row],[Rollover From Last Month]],0)+Budgets[[#This Row],[Total Debits]]-Budgets[[#This Row],[Total Credits]])</f>
-        <v>#N/A</v>
-      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="9" t="e">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Healthcare Deductions]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D7" s="9" t="e">
+      <c r="D7" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Healthcare Deductions]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E7" s="9" t="e">
+      <c r="E7" s="4" t="e">
         <f ca="1">D7-C7</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="9" t="e">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Other Payroll Deductions]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D8" s="9" t="e">
+      <c r="D8" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Other Payroll Deductions]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E8" s="9" t="e">
+      <c r="E8" s="4" t="e">
         <f t="shared" ref="E8" ca="1" si="0">D8-C8</f>
         <v>#N/A</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="9" t="e">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Taxes]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D9" s="8" t="e">
+      <c r="D9" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Taxes]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E9" s="9" t="e">
+      <c r="E9" s="4" t="e">
         <f ca="1">D9-C9</f>
         <v>#N/A</v>
       </c>
@@ -2274,140 +2220,140 @@
         <v>12</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="9" t="e">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Net Income]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D10" s="8" t="e">
+      <c r="D10" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Net Income]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E10" s="9" t="e">
+      <c r="E10" s="4" t="e">
         <f ca="1">D10-C10</f>
         <v>#N/A</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="12" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="9" t="e">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "&lt;&gt;Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Amount]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D13" s="9" t="e">
+      <c r="D13" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "&lt;&gt;Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Total Debits]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E13" s="9" t="e">
+      <c r="E13" s="4" t="e">
         <f ca="1">D13-C13</f>
         <v>#N/A</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="9" t="e">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "=Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Amount]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="D14" s="9" t="e">
+      <c r="D14" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "=Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Total Credits]")) - SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "=Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Total Debits]"))</f>
         <v>#N/A</v>
       </c>
-      <c r="E14" s="9" t="e">
+      <c r="E14" s="4" t="e">
         <f ca="1">D14-C14</f>
         <v>#N/A</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="12"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="9" t="e">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="e">
         <f ca="1">C13+C14</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="9" t="e">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="e">
         <f ca="1">C10-C13-C14</f>
         <v>#N/A</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
       <c r="I16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2415,57 +2361,39 @@
         <v>9</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="8" t="str">
-        <f>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",$J$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline",#REF!, " "))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="L18" s="8" t="str">
-        <f>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",Expected.Income.Dates[[#This Row],[Gross Income]]*$K$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline", Expected.Income.Dates[[#This Row],[Gross Income]]*#REF!, " "))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="M18" s="9" t="str">
-        <f>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",$L$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline",#REF!, " "))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="N18" s="8" t="str">
-        <f>IF(Expected.Income.Dates[[#This Row],[Employer]]="Advantage",$M$14,IF(Expected.Income.Dates[[#This Row],[Employer]]="Saline",#REF!, " "))</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="O18" s="8" t="str">
-        <f>IF(Expected.Income.Dates[[#This Row],[Employer]]&lt;&gt; "", $N$14*(Expected.Income.Dates[[#This Row],[Gross Income]]-Expected.Income.Dates[[#This Row],[Retirement Contributions]]-Expected.Income.Dates[[#This Row],[Healthcare Deductions]]-Expected.Income.Dates[[#This Row],[Other Payroll Deductions]]), "")</f>
-        <v/>
-      </c>
-      <c r="P18" s="8" t="str">
-        <f>IF(Expected.Income.Dates[[#This Row],[Employer]]&lt;&gt;"", Expected.Income.Dates[[#This Row],[Gross Income]]-Expected.Income.Dates[[#This Row],[Retirement Contributions]]-Expected.Income.Dates[[#This Row],[Healthcare Deductions]]-Expected.Income.Dates[[#This Row],[Other Payroll Deductions]]-Expected.Income.Dates[[#This Row],[Taxes]], "")</f>
-        <v/>
-      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -2488,14 +2416,14 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B20" s="5"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="6"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="8"/>
       <c r="I20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
@@ -2503,109 +2431,92 @@
         <v>9</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="I22" s="5"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="8">
-        <f>Actual.Income[[#This Row],[Gross Income]]-Actual.Income[[#This Row],[Retirement Contributions]]-Actual.Income[[#This Row],[Healthcare Deductions]]-Actual.Income[[#This Row],[Other Payroll Deductions]]-Actual.Income[[#This Row],[Taxes]]</f>
-        <v>0</v>
-      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="3"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="Q27" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G20">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="71" priority="20">
       <formula>AND(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[@Category]") &lt;&gt; "Savings", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[@Type]") = "Credit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="21">
+    <cfRule type="expression" dxfId="70" priority="21">
       <formula>AND(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[@Category]") = "Savings", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Transactions[@Type]") = "Debit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="69" priority="9">
       <formula>AND(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[@Type]")="Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[@[Remaining Budget]]")&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="68" priority="10">
       <formula>AND(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[@Type]")="Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[@[Remaining Budget]]")&lt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="67" priority="11">
       <formula>AND(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[@Type]")&lt;&gt;"Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[@[Remaining Budget]]")&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5 E10">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="66" priority="5">
       <formula>E5&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="65" priority="6">
       <formula>E5&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E9">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="64" priority="7">
       <formula>E6&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="63" priority="8">
       <formula>E6&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="62" priority="1">
       <formula>E14&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>E14&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13 E15">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="60" priority="3">
       <formula>E13&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="59" priority="4">
       <formula>E13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6" xr:uid="{2312BBE8-1DD0-41C6-8CBD-2714C5AF8A88}">
-      <formula1>"Rolling,Fixed"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E20" xr:uid="{EB170196-1118-4C97-9161-E86478D49D67}">
-      <formula1>INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Name]")</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10" xr:uid="{F5503B13-D553-4F16-B6F0-33B91A40639B}">
-      <formula1>"Spending,Reserve,Savings,Loan,Safety Net,Retirement"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20" xr:uid="{B05E802A-906F-40D1-9701-2D696BB85752}">
-      <formula1>"Credit,Debit"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="6">

</xml_diff>

<commit_message>
Update the project schema to reflect the new feature roadmap
</commit_message>
<xml_diff>
--- a/Schema/template.xlsx
+++ b/Schema/template.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\React Budget App\Schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\React Budget App\Code\Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C55DCA-760F-44F2-A39E-7B8034D925D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89033F57-C4A7-4CDE-8E4B-EB45C80005BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A682B92-E955-49E4-9CBC-FB857D42C240}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4A682B92-E955-49E4-9CBC-FB857D42C240}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="24" r:id="rId1"/>
+    <sheet name="Overall-Template" sheetId="25" r:id="rId1"/>
+    <sheet name="Month-Template" sheetId="24" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2039,12 +2040,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD344E3-9A6E-44D3-8BC9-D509ADD300ED}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6492320-3C80-4C51-B522-EBAAC3A7C0D3}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,9 +2084,9 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="e" cm="1">
+      <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_xlfn.TEXTAFTER(CELL("filename",A1),"]")</f>
-        <v>#N/A</v>
+        <v>Month-Template</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -2100,15 +2113,15 @@
       </c>
       <c r="C5" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Gross Income]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D5" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Gross Income]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E5" s="4" t="e">
         <f ca="1">D5-C5</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>5</v>
@@ -2141,15 +2154,15 @@
       </c>
       <c r="C6" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Retirement Contributions]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D6" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Retirement Contributions]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E6" s="4" t="e">
         <f ca="1">D6-C6</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -2166,15 +2179,15 @@
       </c>
       <c r="C7" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Healthcare Deductions]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D7" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Healthcare Deductions]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E7" s="4" t="e">
         <f ca="1">D7-C7</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
@@ -2183,15 +2196,15 @@
       </c>
       <c r="C8" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Other Payroll Deductions]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D8" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Other Payroll Deductions]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E8" s="4" t="e">
         <f t="shared" ref="E8" ca="1" si="0">D8-C8</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>19</v>
@@ -2203,15 +2216,15 @@
       </c>
       <c r="C9" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Taxes]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D9" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Taxes]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E9" s="4" t="e">
         <f ca="1">D9-C9</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>5</v>
@@ -2241,15 +2254,15 @@
       </c>
       <c r="C10" s="4" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Expected_Income[Net Income]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D10" s="3" t="e">
         <f ca="1">SUM(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Actual_Income[Net Income]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E10" s="4" t="e">
         <f ca="1">D10-C10</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -2279,15 +2292,15 @@
       </c>
       <c r="C13" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "&lt;&gt;Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Amount]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D13" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "&lt;&gt;Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Total Debits]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E13" s="4" t="e">
         <f ca="1">D13-C13</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>44</v>
@@ -2314,15 +2327,15 @@
       </c>
       <c r="C14" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "=Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Amount]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D14" s="4" t="e">
         <f ca="1">SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "=Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Total Credits]")) - SUMIF(INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Type]"), "=Saving", INDIRECT("_" &amp; SUBSTITUTE($C$2,"-","_") &amp; "\Budgets[Total Debits]"))</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="E14" s="4" t="e">
         <f ca="1">D14-C14</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="8"/>
@@ -2337,7 +2350,7 @@
       </c>
       <c r="C15" s="4" t="e">
         <f ca="1">C13+C14</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2348,7 +2361,7 @@
       </c>
       <c r="C16" s="4" t="e">
         <f ca="1">C10-C13-C14</f>
-        <v>#N/A</v>
+        <v>#REF!</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>

</xml_diff>

<commit_message>
Add model classes and continue work on Data Importer (WIP)
</commit_message>
<xml_diff>
--- a/Schema/template.xlsx
+++ b/Schema/template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\React Budget App\Code\Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3191026-F2C3-4C1A-9E38-4384A101E6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB87993-979A-4CC4-914A-062B18FF5526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4A682B92-E955-49E4-9CBC-FB857D42C240}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A682B92-E955-49E4-9CBC-FB857D42C240}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overall-Template" sheetId="25" r:id="rId1"/>
+    <sheet name="Setup-Template" sheetId="25" r:id="rId1"/>
     <sheet name="Month-Template" sheetId="24" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -175,9 +175,6 @@
     <t>Budget Type</t>
   </si>
   <si>
-    <t>Is Default?</t>
-  </si>
-  <si>
     <t>Budget Name</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>Tax Withholding Amount</t>
   </si>
   <si>
-    <t>Post Tax Deductions</t>
-  </si>
-  <si>
     <t>Starting Balance</t>
   </si>
   <si>
@@ -217,10 +211,16 @@
     <t>Employer Income Rates</t>
   </si>
   <si>
-    <t>Account Mapping</t>
-  </si>
-  <si>
     <t>Payoff Date</t>
+  </si>
+  <si>
+    <t>Override Account Mapping</t>
+  </si>
+  <si>
+    <t>Is Default</t>
+  </si>
+  <si>
+    <t>Post-Tax Deductions</t>
   </si>
 </sst>
 </file>
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,765 +326,291 @@
       <alignment horizontal="right" readingOrder="2"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
     <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFB9EDFF"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
         </bottom>
       </border>
       <protection locked="1" hidden="0"/>
@@ -1125,6 +651,121 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
@@ -1160,6 +801,220 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
@@ -1301,6 +1156,150 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFB9EDFF"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1837,32 +1836,32 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7477D824-16EA-4400-8A4A-A26D94B0BDB2}" name="Date" dataDxfId="49"/>
     <tableColumn id="2" xr3:uid="{4804B0F6-75F9-4C71-82B4-253110B76157}" name="Location" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{5ECA2053-BFE4-4C1D-B7D3-3F5BE41BA416}" name="Description" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{7496558E-9DF8-4A02-8DAB-BF4F75986351}" name="Type" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{C38D712B-2662-4B3B-A13E-3A4F0BC5BFC0}" name="Budget" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E4B36AAC-31DE-4D9F-A319-89D850670D53}" name="Amount" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{EEFB29C7-05A3-4516-B896-F2772B89D26A}" name="Account Mapping" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{BCEA7BB7-5045-42F1-90BB-67A9047CE11B}" name="Credit Card Account" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{D1D41DA6-76CA-4796-94C8-C63F1E1112F4}" name="Payoff Date" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{5ECA2053-BFE4-4C1D-B7D3-3F5BE41BA416}" name="Credit Card Account" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{7496558E-9DF8-4A02-8DAB-BF4F75986351}" name="Payoff Date" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{C38D712B-2662-4B3B-A13E-3A4F0BC5BFC0}" name="Type" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{E4B36AAC-31DE-4D9F-A319-89D850670D53}" name="Amount" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{EEFB29C7-05A3-4516-B896-F2772B89D26A}" name="Description" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{BCEA7BB7-5045-42F1-90BB-67A9047CE11B}" name="Budget" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{D1D41DA6-76CA-4796-94C8-C63F1E1112F4}" name="Override Account Mapping" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{C273FBC6-CF07-4A38-A070-C0C9DFF56067}" name="AccountBalances" displayName="AccountBalances" ref="L21:N22" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{C273FBC6-CF07-4A38-A070-C0C9DFF56067}" name="AccountBalances" displayName="AccountBalances" ref="L21:N22" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="L21:N22" xr:uid="{9874A6B0-EF6A-4DFE-B7B5-17DAD41163E3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9E5C9582-5D2F-4C0A-ADB1-B75EFE305F06}" name="Account Name" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{80AD80A2-4E70-45A8-91C7-AFB3CA3A6FC7}" name="Date" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{AD75D4A6-C383-4C52-858E-D0105EB0DB85}" name="Amount" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{9E5C9582-5D2F-4C0A-ADB1-B75EFE305F06}" name="Account Name" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{80AD80A2-4E70-45A8-91C7-AFB3CA3A6FC7}" name="Date" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{AD75D4A6-C383-4C52-858E-D0105EB0DB85}" name="Amount" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5295C20-1626-4C76-B7F1-5775E8FB9CC8}" name="EmployerIncomeRates" displayName="EmployerIncomeRates" ref="L9:T10" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5295C20-1626-4C76-B7F1-5775E8FB9CC8}" name="EmployerIncomeRates" displayName="EmployerIncomeRates" ref="L9:T10" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="L9:T10" xr:uid="{F5295C20-1626-4C76-B7F1-5775E8FB9CC8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0D648D37-3BFC-4802-9F99-B6A4EDE9FE0D}" name="Employer" dataDxfId="31"/>
@@ -1872,7 +1871,7 @@
     <tableColumn id="8" xr3:uid="{01BC8582-7CD6-45C3-AB58-9704AD9B4935}" name="Pension Contribution Amount" dataDxfId="27"/>
     <tableColumn id="4" xr3:uid="{0CB4F419-FD7E-4B6C-8BBE-EC2CABC7F1C7}" name="Pre-Tax Deductions" dataDxfId="26"/>
     <tableColumn id="5" xr3:uid="{7F7310D7-C7FC-4659-AED7-48C46DE02E0E}" name="Tax Withholding Amount" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{54ABFE45-F89F-46E6-AED9-4869937C027C}" name="Post Tax Deductions" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{54ABFE45-F89F-46E6-AED9-4869937C027C}" name="Post-Tax Deductions" dataDxfId="24"/>
     <tableColumn id="9" xr3:uid="{E047657F-7A1F-4F49-80B9-D1C189C26317}" name="Net Income" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1880,35 +1879,35 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D3820829-36E6-405D-ACD9-A002668F8A02}" name="AccountMappings" displayName="AccountMappings" ref="L17:P18" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D3820829-36E6-405D-ACD9-A002668F8A02}" name="AccountMappings" displayName="AccountMappings" ref="L17:P18" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="L17:P18" xr:uid="{D3820829-36E6-405D-ACD9-A002668F8A02}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D99DA3E3-3648-4D29-9962-77EEED58C93D}" name="Account Name" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{AC04BEFE-28D3-45E3-8F50-86CB8B80D571}" name="Starting Balance" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{10DF22C7-A3CC-44B0-B9F7-200C62A139B1}" name="Budget Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{939BBFDF-23B5-4EFC-8C78-71486716FAE4}" name="Budget Type" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{92A1D4BF-AE6B-40B0-8465-09A750D8F1F8}" name="Is Default?" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{D99DA3E3-3648-4D29-9962-77EEED58C93D}" name="Account Name" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{AC04BEFE-28D3-45E3-8F50-86CB8B80D571}" name="Starting Balance" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{10DF22C7-A3CC-44B0-B9F7-200C62A139B1}" name="Budget Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{939BBFDF-23B5-4EFC-8C78-71486716FAE4}" name="Budget Type" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{92A1D4BF-AE6B-40B0-8465-09A750D8F1F8}" name="Is Default" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{103746B0-AA49-4CFB-A71A-2DA045A6CD51}" name="Incomes" displayName="Incomes" ref="L5:W6" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{103746B0-AA49-4CFB-A71A-2DA045A6CD51}" name="Incomes" displayName="Incomes" ref="L5:W6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="L5:W6" xr:uid="{103746B0-AA49-4CFB-A71A-2DA045A6CD51}"/>
   <tableColumns count="12">
-    <tableColumn id="10" xr3:uid="{CA9FADB5-7CF8-43D5-B723-9B59FA56EEA6}" name="Date" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{D4E8C762-3129-4A64-898F-DBF2FD6CE658}" name="Description" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{ADF2CEA6-3C31-4ED3-AF1D-1AA8A78A002E}" name="Amount" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{8F78F60B-4799-49EE-82DB-CAA8600494BB}" name="Account" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{0F373E56-89E7-4585-9B86-AC15167898FD}" name="Employer" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{65A09419-1CD9-47C9-8246-1373FB6E84CA}" name="Salary Income" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{4B54D368-91E4-4309-98EA-623D45D3B1CC}" name="Additional Taxable Income" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{1CA7458E-D806-41D2-A689-BD542795C169}" name="Retirement Contribution Amount" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{60E67B56-2787-4612-BFF9-A52A070B97F3}" name="Pension Contribution Amount" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{EF0BB2E1-EE25-45E9-9BFB-E18161A621E8}" name="Pre-Tax Deductions" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{897E39D3-EF5F-4F2D-86B5-052E35D9A9E6}" name="Tax Withholding Amount" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{B49F31F3-445E-40DA-A704-F76450927A13}" name="Post Tax Deductions" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{CA9FADB5-7CF8-43D5-B723-9B59FA56EEA6}" name="Date" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{D4E8C762-3129-4A64-898F-DBF2FD6CE658}" name="Description" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{ADF2CEA6-3C31-4ED3-AF1D-1AA8A78A002E}" name="Amount" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{8F78F60B-4799-49EE-82DB-CAA8600494BB}" name="Account" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0F373E56-89E7-4585-9B86-AC15167898FD}" name="Employer" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{65A09419-1CD9-47C9-8246-1373FB6E84CA}" name="Salary Income" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{4B54D368-91E4-4309-98EA-623D45D3B1CC}" name="Additional Taxable Income" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1CA7458E-D806-41D2-A689-BD542795C169}" name="Retirement Contribution Amount" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{60E67B56-2787-4612-BFF9-A52A070B97F3}" name="Pension Contribution Amount" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EF0BB2E1-EE25-45E9-9BFB-E18161A621E8}" name="Pre-Tax Deductions" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{897E39D3-EF5F-4F2D-86B5-052E35D9A9E6}" name="Tax Withholding Amount" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B49F31F3-445E-40DA-A704-F76450927A13}" name="Post-Tax Deductions" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2213,7 +2212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD344E3-9A6E-44D3-8BC9-D509ADD300ED}">
   <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2260,13 +2259,13 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="B2:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="I1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="23" width="25.7109375" customWidth="1"/>
+    <col min="2" max="24" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
@@ -2293,7 +2292,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
@@ -2322,31 +2321,31 @@
         <v>2</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="W5" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
@@ -2366,10 +2365,10 @@
         <v>#REF!</v>
       </c>
       <c r="L6" s="10"/>
-      <c r="M6" s="14"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
@@ -2412,7 +2411,7 @@
         <v>#REF!</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
@@ -2435,25 +2434,25 @@
         <v>31</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R9" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="S9" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>16</v>
@@ -2595,16 +2594,16 @@
         <v>34</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
@@ -2614,8 +2613,8 @@
       <c r="L18" s="5"/>
       <c r="M18" s="8"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="15"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="14"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -2625,25 +2624,25 @@
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
@@ -2651,10 +2650,10 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="14"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="11"/>
       <c r="L20" s="2" t="s">
         <v>13</v>

</xml_diff>